<commit_message>
splitting columns for data clean-up
</commit_message>
<xml_diff>
--- a/Working_Files/Chap 01/01_05/Finding duplicates with CF.xlsx
+++ b/Working_Files/Chap 01/01_05/Finding duplicates with CF.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\linkedin\Desktop\Excel Managing and Analyzing Data (2022)\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\20127\Documents\GitHub\Order\Excel-Managing-and-Analyzing-Data\Working_Files\Chap 01\01_05\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CED1F9C8-F238-45F0-A7E1-B9E67F756DD9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A93AA5CA-B7CD-4321-B99D-E2A7D44CA82A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="806" yWindow="626" windowWidth="19808" windowHeight="11288" xr2:uid="{70C5247B-F288-4D6E-B98C-A535603C673B}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" activeTab="2" xr2:uid="{70C5247B-F288-4D6E-B98C-A535603C673B}"/>
   </bookViews>
   <sheets>
     <sheet name="Names1" sheetId="3" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="159">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="160">
   <si>
     <t>Waukegan, IL 60085</t>
   </si>
@@ -499,9 +499,6 @@
     <t>A, B, C, D</t>
   </si>
   <si>
-    <t>C</t>
-  </si>
-  <si>
     <t>B, C, D</t>
   </si>
   <si>
@@ -515,6 +512,12 @@
   </si>
   <si>
     <t>Students</t>
+  </si>
+  <si>
+    <t>Duplicate Check</t>
+  </si>
+  <si>
+    <t>Dupe Check</t>
   </si>
 </sst>
 </file>
@@ -565,7 +568,38 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="3">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -854,28 +888,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7AA9B814-92B6-4A41-BA6D-706BA409D795}">
-  <dimension ref="B1:C38"/>
+  <dimension ref="B1:C31"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView showGridLines="0" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="19.75" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="19.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.09375" customWidth="1"/>
-    <col min="2" max="2" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.08203125" customWidth="1"/>
+    <col min="2" max="2" width="17.83203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:3" x14ac:dyDescent="0.45">
+    <row r="1" spans="2:3" ht="20.25" x14ac:dyDescent="0.3">
       <c r="B1" s="1" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="2" spans="2:3" x14ac:dyDescent="0.45">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="2" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>83</v>
       </c>
@@ -883,581 +917,695 @@
         <v>152</v>
       </c>
     </row>
-    <row r="3" spans="2:3" x14ac:dyDescent="0.45">
+    <row r="3" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="C3" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>76</v>
+        <v>82</v>
       </c>
       <c r="C4" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="5" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>78</v>
+      </c>
+      <c r="C5" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="6" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>71</v>
+      </c>
+      <c r="C6" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="7" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="8" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="9" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="10" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>79</v>
+      </c>
+      <c r="C10" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="11" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="12" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>63</v>
+      </c>
+      <c r="C12" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B5" t="s">
-        <v>76</v>
-      </c>
-      <c r="C5" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B6" t="s">
-        <v>82</v>
-      </c>
-      <c r="C6" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="7" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B7" t="s">
-        <v>78</v>
-      </c>
-      <c r="C7" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="8" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B8" t="s">
-        <v>71</v>
-      </c>
-      <c r="C8" t="s">
+    <row r="13" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="14" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>77</v>
+      </c>
+      <c r="C14" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="9" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B9" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="10" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B10" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="11" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B11" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="12" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B12" t="s">
-        <v>79</v>
-      </c>
-      <c r="C12" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="13" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B13" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="14" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B14" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="15" spans="2:3" x14ac:dyDescent="0.45">
+    <row r="15" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="16" spans="2:3" x14ac:dyDescent="0.45">
+        <v>67</v>
+      </c>
+      <c r="C15" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="16" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
-        <v>63</v>
-      </c>
-      <c r="C16" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
+        <v>91</v>
+      </c>
+      <c r="C18" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B17" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B18" t="s">
-        <v>77</v>
-      </c>
-      <c r="C18" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.45">
+    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
-        <v>67</v>
-      </c>
-      <c r="C19" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="20" spans="2:3" x14ac:dyDescent="0.45">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
-        <v>67</v>
-      </c>
-      <c r="C20" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="21" spans="2:3" x14ac:dyDescent="0.45">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="22" spans="2:3" x14ac:dyDescent="0.45">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="22" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="23" spans="2:3" x14ac:dyDescent="0.45">
+        <v>73</v>
+      </c>
+      <c r="C22" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="23" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
-        <v>91</v>
-      </c>
-      <c r="C23" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="24" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B24" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="25" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B25" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="26" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B26" t="s">
+        <v>86</v>
+      </c>
+      <c r="C26" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="24" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B24" t="s">
-        <v>91</v>
-      </c>
-      <c r="C24" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="25" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B25" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="26" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B26" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="27" spans="2:3" x14ac:dyDescent="0.45">
+    <row r="27" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="28" spans="2:3" x14ac:dyDescent="0.45">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="28" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
-        <v>73</v>
-      </c>
-      <c r="C28" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="29" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B29" t="s">
+        <v>64</v>
+      </c>
+      <c r="C29" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="29" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B29" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="30" spans="2:3" x14ac:dyDescent="0.45">
+    <row r="30" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="31" spans="2:3" x14ac:dyDescent="0.45">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="31" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="32" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B32" t="s">
-        <v>86</v>
-      </c>
-      <c r="C32" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="33" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B33" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="34" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B34" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="35" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B35" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="36" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B36" t="s">
-        <v>64</v>
-      </c>
-      <c r="C36" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="37" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B37" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="38" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B38" t="s">
         <v>90</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B2:B38">
-    <sortCondition ref="B7:B38"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B2:B31">
+    <sortCondition ref="B5:B31"/>
   </sortState>
+  <conditionalFormatting sqref="B1:B1048576">
+    <cfRule type="duplicateValues" dxfId="2" priority="1"/>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C001667-3E06-40E0-AD59-42D9F95AF13E}">
-  <dimension ref="B1:C38"/>
+  <dimension ref="B1:D38"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="D1" sqref="D1:D1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="19.75" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="19.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="10.90234375" customWidth="1"/>
+    <col min="2" max="2" width="10.9140625" customWidth="1"/>
     <col min="3" max="3" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.4140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:3" x14ac:dyDescent="0.45">
+    <row r="1" spans="2:4" ht="20.25" x14ac:dyDescent="0.3">
       <c r="B1" s="1" t="s">
         <v>147</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>148</v>
       </c>
-    </row>
-    <row r="2" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="D1" s="1" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="2" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>93</v>
       </c>
       <c r="C2" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="3" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="D2" t="str">
+        <f>B2&amp;C2</f>
+        <v>AliceLakatos</v>
+      </c>
+    </row>
+    <row r="3" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>94</v>
       </c>
       <c r="C3" t="s">
         <v>121</v>
       </c>
-    </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="D3" t="str">
+        <f t="shared" ref="D3:D38" si="0">B3&amp;C3</f>
+        <v>BernardEvans</v>
+      </c>
+    </row>
+    <row r="4" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>95</v>
       </c>
       <c r="C4" t="s">
         <v>122</v>
       </c>
-    </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="D4" t="str">
+        <f t="shared" si="0"/>
+        <v>CierraCalderon</v>
+      </c>
+    </row>
+    <row r="5" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>96</v>
       </c>
       <c r="C5" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="D5" t="str">
+        <f t="shared" si="0"/>
+        <v>ClintHurst</v>
+      </c>
+    </row>
+    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>97</v>
       </c>
       <c r="C6" t="s">
         <v>124</v>
       </c>
-    </row>
-    <row r="7" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="D6" t="str">
+        <f t="shared" si="0"/>
+        <v>DorothyKerr</v>
+      </c>
+    </row>
+    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>98</v>
       </c>
       <c r="C7" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="8" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="D7" t="str">
+        <f t="shared" si="0"/>
+        <v>FloridaBrandt</v>
+      </c>
+    </row>
+    <row r="8" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>99</v>
       </c>
       <c r="C8" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="9" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="D8" t="str">
+        <f t="shared" si="0"/>
+        <v>FrançoisParrish</v>
+      </c>
+    </row>
+    <row r="9" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>94</v>
       </c>
       <c r="C9" t="s">
         <v>121</v>
       </c>
-    </row>
-    <row r="10" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="D9" t="str">
+        <f t="shared" si="0"/>
+        <v>BernardEvans</v>
+      </c>
+    </row>
+    <row r="10" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>100</v>
       </c>
       <c r="C10" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="11" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="D10" t="str">
+        <f t="shared" si="0"/>
+        <v>CecilyParrish</v>
+      </c>
+    </row>
+    <row r="11" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>99</v>
       </c>
       <c r="C11" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="12" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="D11" t="str">
+        <f t="shared" si="0"/>
+        <v>FrançoisParrish</v>
+      </c>
+    </row>
+    <row r="12" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>99</v>
       </c>
       <c r="C12" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="13" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="D12" t="str">
+        <f t="shared" si="0"/>
+        <v>FrançoisParrish</v>
+      </c>
+    </row>
+    <row r="13" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>101</v>
       </c>
       <c r="C13" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="14" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="D13" t="str">
+        <f t="shared" si="0"/>
+        <v>ErikaParrish</v>
+      </c>
+    </row>
+    <row r="14" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>102</v>
       </c>
       <c r="C14" t="s">
         <v>127</v>
       </c>
-    </row>
-    <row r="15" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="D14" t="str">
+        <f t="shared" si="0"/>
+        <v>GillianHerrera</v>
+      </c>
+    </row>
+    <row r="15" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>103</v>
       </c>
       <c r="C15" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="16" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="D15" t="str">
+        <f t="shared" si="0"/>
+        <v>HortenciaBaker</v>
+      </c>
+    </row>
+    <row r="16" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>103</v>
       </c>
       <c r="C16" t="s">
         <v>129</v>
       </c>
-    </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="D16" t="str">
+        <f t="shared" si="0"/>
+        <v>HortenciaWallace</v>
+      </c>
+    </row>
+    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>103</v>
       </c>
       <c r="C17" t="s">
         <v>129</v>
       </c>
-    </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="D17" t="str">
+        <f t="shared" si="0"/>
+        <v>HortenciaWallace</v>
+      </c>
+    </row>
+    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
         <v>94</v>
       </c>
       <c r="C18" t="s">
         <v>121</v>
       </c>
-    </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="D18" t="str">
+        <f t="shared" si="0"/>
+        <v>BernardEvans</v>
+      </c>
+    </row>
+    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
         <v>104</v>
       </c>
       <c r="C19" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="20" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="D19" t="str">
+        <f t="shared" si="0"/>
+        <v>IreneArroyo</v>
+      </c>
+    </row>
+    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
         <v>105</v>
       </c>
       <c r="C20" t="s">
         <v>131</v>
       </c>
-    </row>
-    <row r="21" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="D20" t="str">
+        <f t="shared" si="0"/>
+        <v>JeanSeys</v>
+      </c>
+    </row>
+    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
         <v>106</v>
       </c>
       <c r="C21" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="22" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="D21" t="str">
+        <f t="shared" si="0"/>
+        <v>JoãoIbanez</v>
+      </c>
+    </row>
+    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
         <v>106</v>
       </c>
       <c r="C22" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="23" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="D22" t="str">
+        <f t="shared" si="0"/>
+        <v>JoãoIbanez</v>
+      </c>
+    </row>
+    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
         <v>107</v>
       </c>
       <c r="C23" t="s">
         <v>133</v>
       </c>
-    </row>
-    <row r="24" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="D23" t="str">
+        <f t="shared" si="0"/>
+        <v>KarriArlotta</v>
+      </c>
+    </row>
+    <row r="24" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
         <v>108</v>
       </c>
       <c r="C24" t="s">
         <v>134</v>
       </c>
-    </row>
-    <row r="25" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="D24" t="str">
+        <f t="shared" si="0"/>
+        <v>KekoaSrinivas</v>
+      </c>
+    </row>
+    <row r="25" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
         <v>109</v>
       </c>
       <c r="C25" t="s">
         <v>135</v>
       </c>
-    </row>
-    <row r="26" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="D25" t="str">
+        <f t="shared" si="0"/>
+        <v>LeahSanford</v>
+      </c>
+    </row>
+    <row r="26" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
         <v>110</v>
       </c>
       <c r="C26" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="27" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="D26" t="str">
+        <f t="shared" si="0"/>
+        <v>MarioNemecek</v>
+      </c>
+    </row>
+    <row r="27" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
         <v>111</v>
       </c>
       <c r="C27" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="28" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="D27" t="str">
+        <f t="shared" si="0"/>
+        <v>MaslinPaci</v>
+      </c>
+    </row>
+    <row r="28" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
         <v>101</v>
       </c>
       <c r="C28" t="s">
         <v>138</v>
       </c>
-    </row>
-    <row r="29" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="D28" t="str">
+        <f t="shared" si="0"/>
+        <v>ErikaNewton</v>
+      </c>
+    </row>
+    <row r="29" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
         <v>112</v>
       </c>
       <c r="C29" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="30" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="D29" t="str">
+        <f t="shared" si="0"/>
+        <v>NatashaStill</v>
+      </c>
+    </row>
+    <row r="30" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
         <v>113</v>
       </c>
       <c r="C30" t="s">
         <v>140</v>
       </c>
-    </row>
-    <row r="31" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="D30" t="str">
+        <f t="shared" si="0"/>
+        <v>RhettRossi</v>
+      </c>
+    </row>
+    <row r="31" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
         <v>114</v>
       </c>
       <c r="C31" t="s">
         <v>141</v>
       </c>
-    </row>
-    <row r="32" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="D31" t="str">
+        <f t="shared" si="0"/>
+        <v>RichChauvaine</v>
+      </c>
+    </row>
+    <row r="32" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
         <v>115</v>
       </c>
       <c r="C32" t="s">
         <v>142</v>
       </c>
-    </row>
-    <row r="33" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="D32" t="str">
+        <f t="shared" si="0"/>
+        <v>ShamikaNeuheuser</v>
+      </c>
+    </row>
+    <row r="33" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
         <v>116</v>
       </c>
       <c r="C33" t="s">
         <v>135</v>
       </c>
-    </row>
-    <row r="34" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="D33" t="str">
+        <f t="shared" si="0"/>
+        <v>SusanneSanford</v>
+      </c>
+    </row>
+    <row r="34" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
         <v>117</v>
       </c>
       <c r="C34" t="s">
         <v>143</v>
       </c>
-    </row>
-    <row r="35" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="D34" t="str">
+        <f t="shared" si="0"/>
+        <v>TempestNazaire</v>
+      </c>
+    </row>
+    <row r="35" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
         <v>118</v>
       </c>
       <c r="C35" t="s">
         <v>144</v>
       </c>
-    </row>
-    <row r="36" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="D35" t="str">
+        <f t="shared" si="0"/>
+        <v>VellSpencer</v>
+      </c>
+    </row>
+    <row r="36" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
         <v>119</v>
       </c>
       <c r="C36" t="s">
         <v>145</v>
       </c>
-    </row>
-    <row r="37" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="D36" t="str">
+        <f t="shared" si="0"/>
+        <v>YarinAusten</v>
+      </c>
+    </row>
+    <row r="37" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
         <v>94</v>
       </c>
       <c r="C37" t="s">
         <v>146</v>
       </c>
-    </row>
-    <row r="38" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="D37" t="str">
+        <f t="shared" si="0"/>
+        <v>BernardTolan</v>
+      </c>
+    </row>
+    <row r="38" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
         <v>114</v>
       </c>
       <c r="C38" t="s">
         <v>141</v>
       </c>
+      <c r="D38" t="str">
+        <f t="shared" si="0"/>
+        <v>RichChauvaine</v>
+      </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="D1:D1048576">
+    <cfRule type="duplicateValues" dxfId="1" priority="1"/>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{45FF8729-EBCD-4914-A0EA-6D0C65DBCA4E}">
-  <dimension ref="B1:E21"/>
+  <dimension ref="B1:F21"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A13" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="C1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="19.75" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="19.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.046875" customWidth="1"/>
-    <col min="2" max="2" width="13.046875" customWidth="1"/>
-    <col min="3" max="3" width="12.7109375" customWidth="1"/>
-    <col min="4" max="4" width="23.47265625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="22.140625" customWidth="1"/>
-    <col min="6" max="6" width="31.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.08203125" customWidth="1"/>
+    <col min="2" max="2" width="13.08203125" customWidth="1"/>
+    <col min="3" max="3" width="12.75" customWidth="1"/>
+    <col min="4" max="4" width="23.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22.1640625" customWidth="1"/>
+    <col min="6" max="6" width="31.25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="1" spans="2:6" ht="20.25" x14ac:dyDescent="0.3">
       <c r="B1" s="1" t="s">
         <v>62</v>
       </c>
@@ -1470,8 +1618,11 @@
       <c r="E1" s="1" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="2" spans="2:5" x14ac:dyDescent="0.45">
+      <c r="F1" s="1" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="2" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>31</v>
       </c>
@@ -1484,8 +1635,12 @@
       <c r="E2" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="3" spans="2:5" x14ac:dyDescent="0.45">
+      <c r="F2" t="str">
+        <f>LEFT(B2,3)&amp;LEFT(C2,2)&amp;MID(D2,2,4)&amp;RIGHT(E2,3)</f>
+        <v>EvaNo08 W635</v>
+      </c>
+    </row>
+    <row r="3" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>48</v>
       </c>
@@ -1498,8 +1653,12 @@
       <c r="E3" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.45">
+      <c r="F3" t="str">
+        <f t="shared" ref="F3:F21" si="0">LEFT(B3,3)&amp;LEFT(C3,2)&amp;MID(D3,2,4)&amp;RIGHT(E3,3)</f>
+        <v>HapSi415 734</v>
+      </c>
+    </row>
+    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>51</v>
       </c>
@@ -1512,8 +1671,12 @@
       <c r="E4" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.45">
+      <c r="F4" t="str">
+        <f t="shared" si="0"/>
+        <v>TobRa004 236</v>
+      </c>
+    </row>
+    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>53</v>
       </c>
@@ -1526,8 +1689,12 @@
       <c r="E5" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.45">
+      <c r="F5" t="str">
+        <f t="shared" si="0"/>
+        <v>AmyRa004 236</v>
+      </c>
+    </row>
+    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>3</v>
       </c>
@@ -1540,8 +1707,12 @@
       <c r="E6" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.45">
+      <c r="F6" t="str">
+        <f t="shared" si="0"/>
+        <v>JohWa004 236</v>
+      </c>
+    </row>
+    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>3</v>
       </c>
@@ -1554,8 +1725,12 @@
       <c r="E7" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="8" spans="2:5" x14ac:dyDescent="0.45">
+      <c r="F7" t="str">
+        <f t="shared" si="0"/>
+        <v>JohWa068 011</v>
+      </c>
+    </row>
+    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>11</v>
       </c>
@@ -1568,8 +1743,12 @@
       <c r="E8" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="9" spans="2:5" x14ac:dyDescent="0.45">
+      <c r="F8" t="str">
+        <f t="shared" si="0"/>
+        <v>MoiMa1110458</v>
+      </c>
+    </row>
+    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>37</v>
       </c>
@@ -1582,8 +1761,12 @@
       <c r="E9" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="10" spans="2:5" x14ac:dyDescent="0.45">
+      <c r="F9" t="str">
+        <f t="shared" si="0"/>
+        <v>LeoSi3923830</v>
+      </c>
+    </row>
+    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>19</v>
       </c>
@@ -1596,8 +1779,12 @@
       <c r="E10" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="11" spans="2:5" x14ac:dyDescent="0.45">
+      <c r="F10" t="str">
+        <f t="shared" si="0"/>
+        <v>WayMc41 N156</v>
+      </c>
+    </row>
+    <row r="11" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>23</v>
       </c>
@@ -1610,8 +1797,12 @@
       <c r="E11" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="12" spans="2:5" x14ac:dyDescent="0.45">
+      <c r="F11" t="str">
+        <f t="shared" si="0"/>
+        <v>AlfRo SW 922</v>
+      </c>
+    </row>
+    <row r="12" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>42</v>
       </c>
@@ -1624,8 +1815,12 @@
       <c r="E12" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="13" spans="2:5" x14ac:dyDescent="0.45">
+      <c r="F12" t="str">
+        <f t="shared" si="0"/>
+        <v>ChaLe5 Ad081</v>
+      </c>
+    </row>
+    <row r="13" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>42</v>
       </c>
@@ -1638,8 +1833,12 @@
       <c r="E13" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="14" spans="2:5" x14ac:dyDescent="0.45">
+      <c r="F13" t="str">
+        <f t="shared" si="0"/>
+        <v>ChaLe5 Ad081</v>
+      </c>
+    </row>
+    <row r="14" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>42</v>
       </c>
@@ -1652,8 +1851,12 @@
       <c r="E14" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="15" spans="2:5" x14ac:dyDescent="0.45">
+      <c r="F14" t="str">
+        <f t="shared" si="0"/>
+        <v>ChaLe5 Ad081</v>
+      </c>
+    </row>
+    <row r="15" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>149</v>
       </c>
@@ -1666,8 +1869,12 @@
       <c r="E15" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="16" spans="2:5" x14ac:dyDescent="0.45">
+      <c r="F15" t="str">
+        <f t="shared" si="0"/>
+        <v>JohLe5 Ad081</v>
+      </c>
+    </row>
+    <row r="16" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>27</v>
       </c>
@@ -1680,8 +1887,12 @@
       <c r="E16" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.45">
+      <c r="F16" t="str">
+        <f t="shared" si="0"/>
+        <v>CynGr50 S708</v>
+      </c>
+    </row>
+    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>3</v>
       </c>
@@ -1694,8 +1905,12 @@
       <c r="E17" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.45">
+      <c r="F17" t="str">
+        <f t="shared" si="0"/>
+        <v>JohWa11 W085</v>
+      </c>
+    </row>
+    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
         <v>57</v>
       </c>
@@ -1708,8 +1923,12 @@
       <c r="E18" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.45">
+      <c r="F18" t="str">
+        <f t="shared" si="0"/>
+        <v>TodBi521 014</v>
+      </c>
+    </row>
+    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
         <v>57</v>
       </c>
@@ -1722,8 +1941,12 @@
       <c r="E19" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.45">
+      <c r="F19" t="str">
+        <f t="shared" si="0"/>
+        <v>TodBi521 014</v>
+      </c>
+    </row>
+    <row r="20" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
         <v>15</v>
       </c>
@@ -1736,8 +1959,12 @@
       <c r="E20" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.45">
+      <c r="F20" t="str">
+        <f t="shared" si="0"/>
+        <v>LarMa2 Up554</v>
+      </c>
+    </row>
+    <row r="21" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
         <v>7</v>
       </c>
@@ -1749,12 +1976,19 @@
       </c>
       <c r="E21" t="s">
         <v>4</v>
+      </c>
+      <c r="F21" t="str">
+        <f t="shared" si="0"/>
+        <v>AleLi5 Ol453</v>
       </c>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B2:E21">
     <sortCondition ref="D3:D21"/>
   </sortState>
+  <conditionalFormatting sqref="F1:F1048576">
+    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>